<commit_message>
ultimos cambios en casa
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\geo-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB4346C-D741-4BF4-9640-8492D94087AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E2735E-C367-4408-8D49-A4A62E4A91D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{309DB08E-BE09-4144-A5B9-FEAA5A4D9983}"/>
   </bookViews>
@@ -698,2114 +698,1799 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659E6E70-F2D6-4149-8147-FCFCF5A4587D}">
-  <dimension ref="A2:G106"/>
+  <dimension ref="A2:F106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G106"/>
+      <selection activeCell="D68" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="38.5546875" customWidth="1"/>
+    <col min="4" max="4" width="38.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
         <v>105</v>
       </c>
       <c r="F2" t="s">
         <v>105</v>
       </c>
-      <c r="G2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" t="s">
         <v>105</v>
       </c>
       <c r="F3" t="s">
         <v>105</v>
       </c>
-      <c r="G3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" t="s">
         <v>105</v>
       </c>
       <c r="F4" t="s">
         <v>105</v>
       </c>
-      <c r="G4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" t="s">
         <v>105</v>
       </c>
       <c r="F5" t="s">
         <v>105</v>
       </c>
-      <c r="G5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" t="s">
         <v>105</v>
       </c>
       <c r="F6" t="s">
         <v>105</v>
       </c>
-      <c r="G6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="D7" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" t="s">
         <v>105</v>
       </c>
       <c r="F7" t="s">
         <v>105</v>
       </c>
-      <c r="G7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="D8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" t="s">
         <v>105</v>
       </c>
       <c r="F8" t="s">
         <v>105</v>
       </c>
-      <c r="G8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="D9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E9" t="s">
         <v>105</v>
       </c>
       <c r="F9" t="s">
         <v>105</v>
       </c>
-      <c r="G9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="D10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" t="s">
         <v>105</v>
       </c>
       <c r="F10" t="s">
         <v>105</v>
       </c>
-      <c r="G10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="D11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" t="s">
         <v>105</v>
       </c>
       <c r="F11" t="s">
         <v>105</v>
       </c>
-      <c r="G11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="D12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E12" t="s">
         <v>105</v>
       </c>
       <c r="F12" t="s">
         <v>105</v>
       </c>
-      <c r="G12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="D13" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13" t="s">
         <v>105</v>
       </c>
       <c r="F13" t="s">
         <v>105</v>
       </c>
-      <c r="G13" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="D14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" t="s">
         <v>105</v>
       </c>
       <c r="F14" t="s">
         <v>105</v>
       </c>
-      <c r="G14" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" t="s">
         <v>105</v>
       </c>
       <c r="F15" t="s">
         <v>105</v>
       </c>
-      <c r="G15" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="D16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" t="s">
         <v>105</v>
       </c>
       <c r="F16" t="s">
         <v>105</v>
       </c>
-      <c r="G16" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" s="2" t="s">
+      <c r="D17" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" t="s">
         <v>105</v>
       </c>
       <c r="F17" t="s">
         <v>105</v>
       </c>
-      <c r="G17" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" s="2" t="s">
+      <c r="D18" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" t="s">
         <v>105</v>
       </c>
       <c r="F18" t="s">
         <v>105</v>
       </c>
-      <c r="G18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19" s="2" t="s">
+      <c r="D19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" t="s">
         <v>105</v>
       </c>
       <c r="F19" t="s">
         <v>105</v>
       </c>
-      <c r="G19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20" s="2" t="s">
+      <c r="D20" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" t="s">
         <v>105</v>
       </c>
       <c r="F20" t="s">
         <v>105</v>
       </c>
-      <c r="G20" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" s="2" t="s">
+      <c r="D21" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" t="s">
         <v>105</v>
       </c>
       <c r="F21" t="s">
         <v>105</v>
       </c>
-      <c r="G21" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22" s="2" t="s">
+      <c r="D22" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" t="s">
         <v>105</v>
       </c>
       <c r="F22" t="s">
         <v>105</v>
       </c>
-      <c r="G22" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" s="2" t="s">
+      <c r="D23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E23" t="s">
         <v>105</v>
       </c>
       <c r="F23" t="s">
         <v>105</v>
       </c>
-      <c r="G23" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24" s="2" t="s">
+      <c r="D24" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E24" t="s">
         <v>105</v>
       </c>
       <c r="F24" t="s">
         <v>105</v>
       </c>
-      <c r="G24" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" s="2" t="s">
+      <c r="D25" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E25" t="s">
         <v>105</v>
       </c>
       <c r="F25" t="s">
         <v>105</v>
       </c>
-      <c r="G25" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26" s="2" t="s">
+      <c r="D26" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" t="s">
         <v>105</v>
       </c>
       <c r="F26" t="s">
         <v>105</v>
       </c>
-      <c r="G26" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" s="2" t="s">
+      <c r="D27" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E27" t="s">
         <v>105</v>
       </c>
       <c r="F27" t="s">
         <v>105</v>
       </c>
-      <c r="G27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" s="2" t="s">
+      <c r="D28" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E28" t="s">
         <v>105</v>
       </c>
       <c r="F28" t="s">
         <v>105</v>
       </c>
-      <c r="G28" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29" s="2" t="s">
+      <c r="D29" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" t="s">
         <v>105</v>
       </c>
       <c r="F29" t="s">
         <v>105</v>
       </c>
-      <c r="G29" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30" s="2" t="s">
+      <c r="D30" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" t="s">
         <v>105</v>
       </c>
       <c r="F30" t="s">
         <v>105</v>
       </c>
-      <c r="G30" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31" s="2" t="s">
+      <c r="D31" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" t="s">
         <v>105</v>
       </c>
       <c r="F31" t="s">
         <v>105</v>
       </c>
-      <c r="G31" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32" s="2" t="s">
+      <c r="D32" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E32" t="s">
         <v>105</v>
       </c>
       <c r="F32" t="s">
         <v>105</v>
       </c>
-      <c r="G32" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33" s="2" t="s">
+      <c r="D33" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E33" t="s">
         <v>105</v>
       </c>
       <c r="F33" t="s">
         <v>105</v>
       </c>
-      <c r="G33" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34" s="2" t="s">
+      <c r="D34" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E34" t="s">
         <v>105</v>
       </c>
       <c r="F34" t="s">
         <v>105</v>
       </c>
-      <c r="G34" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35" s="2" t="s">
+      <c r="D35" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E35" t="s">
         <v>105</v>
       </c>
       <c r="F35" t="s">
         <v>105</v>
       </c>
-      <c r="G35" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36" s="2" t="s">
+      <c r="D36" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E36" t="s">
         <v>105</v>
       </c>
       <c r="F36" t="s">
         <v>105</v>
       </c>
-      <c r="G36" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37" s="2" t="s">
+      <c r="D37" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E37" t="s">
         <v>105</v>
       </c>
       <c r="F37" t="s">
         <v>105</v>
       </c>
-      <c r="G37" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38" s="2" t="s">
+      <c r="D38" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E38" t="s">
         <v>105</v>
       </c>
       <c r="F38" t="s">
         <v>105</v>
       </c>
-      <c r="G38" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39" s="2" t="s">
+      <c r="D39" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E39" t="s">
         <v>105</v>
       </c>
       <c r="F39" t="s">
         <v>105</v>
       </c>
-      <c r="G39" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40" s="2" t="s">
+      <c r="D40" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E40" t="s">
         <v>105</v>
       </c>
       <c r="F40" t="s">
         <v>105</v>
       </c>
-      <c r="G40" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41" s="2" t="s">
+      <c r="D41" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E41" t="s">
         <v>105</v>
       </c>
       <c r="F41" t="s">
         <v>105</v>
       </c>
-      <c r="G41" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D42">
-        <v>1</v>
-      </c>
-      <c r="E42" s="2" t="s">
+      <c r="D42" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E42" t="s">
         <v>105</v>
       </c>
       <c r="F42" t="s">
         <v>105</v>
       </c>
-      <c r="G42" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D43">
-        <v>1</v>
-      </c>
-      <c r="E43" s="2" t="s">
+      <c r="D43" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E43" t="s">
         <v>105</v>
       </c>
       <c r="F43" t="s">
         <v>105</v>
       </c>
-      <c r="G43" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44" s="2" t="s">
+      <c r="D44" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E44" t="s">
         <v>105</v>
       </c>
       <c r="F44" t="s">
         <v>105</v>
       </c>
-      <c r="G44" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D45">
-        <v>1</v>
-      </c>
-      <c r="E45" s="2" t="s">
+      <c r="D45" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E45" t="s">
         <v>105</v>
       </c>
       <c r="F45" t="s">
         <v>105</v>
       </c>
-      <c r="G45" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-      <c r="E46" s="2" t="s">
+      <c r="D46" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E46" t="s">
         <v>105</v>
       </c>
       <c r="F46" t="s">
         <v>105</v>
       </c>
-      <c r="G46" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D47">
-        <v>1</v>
-      </c>
-      <c r="E47" s="2" t="s">
+      <c r="D47" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E47" t="s">
         <v>105</v>
       </c>
       <c r="F47" t="s">
         <v>105</v>
       </c>
-      <c r="G47" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-      <c r="E48" s="2" t="s">
+      <c r="D48" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E48" t="s">
         <v>105</v>
       </c>
       <c r="F48" t="s">
         <v>105</v>
       </c>
-      <c r="G48" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="E49" s="2" t="s">
+      <c r="D49" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E49" t="s">
         <v>105</v>
       </c>
       <c r="F49" t="s">
         <v>105</v>
       </c>
-      <c r="G49" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D50">
-        <v>1</v>
-      </c>
-      <c r="E50" s="2" t="s">
+      <c r="D50" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E50" t="s">
         <v>105</v>
       </c>
       <c r="F50" t="s">
         <v>105</v>
       </c>
-      <c r="G50" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-      <c r="E51" s="2" t="s">
+      <c r="D51" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E51" t="s">
         <v>105</v>
       </c>
       <c r="F51" t="s">
         <v>105</v>
       </c>
-      <c r="G51" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-      <c r="E52" s="2" t="s">
+      <c r="D52" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E52" t="s">
         <v>105</v>
       </c>
       <c r="F52" t="s">
         <v>105</v>
       </c>
-      <c r="G52" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D53">
-        <v>1</v>
-      </c>
-      <c r="E53" s="2" t="s">
+      <c r="D53" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E53" t="s">
         <v>105</v>
       </c>
       <c r="F53" t="s">
         <v>105</v>
       </c>
-      <c r="G53" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D54">
-        <v>1</v>
-      </c>
-      <c r="E54" s="2" t="s">
+      <c r="D54" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E54" t="s">
         <v>105</v>
       </c>
       <c r="F54" t="s">
         <v>105</v>
       </c>
-      <c r="G54" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D55">
-        <v>1</v>
-      </c>
-      <c r="E55" s="2" t="s">
+      <c r="D55" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E55" t="s">
         <v>105</v>
       </c>
       <c r="F55" t="s">
         <v>105</v>
       </c>
-      <c r="G55" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D56">
-        <v>1</v>
-      </c>
-      <c r="E56" s="2" t="s">
+      <c r="D56" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E56" t="s">
         <v>105</v>
       </c>
       <c r="F56" t="s">
         <v>105</v>
       </c>
-      <c r="G56" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D57">
-        <v>1</v>
-      </c>
-      <c r="E57" s="2" t="s">
+      <c r="D57" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E57" t="s">
         <v>105</v>
       </c>
       <c r="F57" t="s">
         <v>105</v>
       </c>
-      <c r="G57" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D58">
-        <v>1</v>
-      </c>
-      <c r="E58" s="2" t="s">
+      <c r="D58" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E58" t="s">
         <v>105</v>
       </c>
       <c r="F58" t="s">
         <v>105</v>
       </c>
-      <c r="G58" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D59">
-        <v>1</v>
-      </c>
-      <c r="E59" s="2" t="s">
+      <c r="D59" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E59" t="s">
         <v>105</v>
       </c>
       <c r="F59" t="s">
         <v>105</v>
       </c>
-      <c r="G59" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="E60" s="2" t="s">
+      <c r="D60" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E60" t="s">
         <v>105</v>
       </c>
       <c r="F60" t="s">
         <v>105</v>
       </c>
-      <c r="G60" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D61">
-        <v>1</v>
-      </c>
-      <c r="E61" s="2" t="s">
+      <c r="D61" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E61" t="s">
         <v>105</v>
       </c>
       <c r="F61" t="s">
         <v>105</v>
       </c>
-      <c r="G61" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D62">
-        <v>1</v>
-      </c>
-      <c r="E62" s="2" t="s">
+      <c r="D62" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E62" t="s">
         <v>105</v>
       </c>
       <c r="F62" t="s">
         <v>105</v>
       </c>
-      <c r="G62" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D63">
-        <v>1</v>
-      </c>
-      <c r="E63" s="2" t="s">
+      <c r="D63" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E63" t="s">
         <v>105</v>
       </c>
       <c r="F63" t="s">
         <v>105</v>
       </c>
-      <c r="G63" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D64">
-        <v>1</v>
-      </c>
-      <c r="E64" s="2" t="s">
+      <c r="D64" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E64" t="s">
         <v>105</v>
       </c>
       <c r="F64" t="s">
         <v>105</v>
       </c>
-      <c r="G64" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D65">
-        <v>1</v>
-      </c>
-      <c r="E65" s="2" t="s">
+      <c r="D65" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E65" t="s">
         <v>105</v>
       </c>
       <c r="F65" t="s">
         <v>105</v>
       </c>
-      <c r="G65" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D66">
-        <v>1</v>
-      </c>
-      <c r="E66" s="2" t="s">
+      <c r="D66" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E66" t="s">
         <v>105</v>
       </c>
       <c r="F66" t="s">
         <v>105</v>
       </c>
-      <c r="G66" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D67">
-        <v>1</v>
-      </c>
-      <c r="E67" s="2" t="s">
+      <c r="D67" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E67" t="s">
         <v>105</v>
       </c>
       <c r="F67" t="s">
         <v>105</v>
       </c>
-      <c r="G67" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D68">
-        <v>1</v>
-      </c>
-      <c r="E68" s="2" t="s">
+      <c r="D68" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E68" t="s">
         <v>105</v>
       </c>
       <c r="F68" t="s">
         <v>105</v>
       </c>
-      <c r="G68" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D69">
-        <v>1</v>
-      </c>
-      <c r="E69" s="2" t="s">
+      <c r="D69" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E69" t="s">
         <v>105</v>
       </c>
       <c r="F69" t="s">
         <v>105</v>
       </c>
-      <c r="G69" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D70">
-        <v>1</v>
-      </c>
-      <c r="E70" s="2" t="s">
+      <c r="D70" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E70" t="s">
         <v>105</v>
       </c>
       <c r="F70" t="s">
         <v>105</v>
       </c>
-      <c r="G70" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D71">
-        <v>1</v>
-      </c>
-      <c r="E71" s="2" t="s">
+      <c r="D71" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E71" t="s">
         <v>105</v>
       </c>
       <c r="F71" t="s">
         <v>105</v>
       </c>
-      <c r="G71" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D72">
-        <v>1</v>
-      </c>
-      <c r="E72" s="2" t="s">
+      <c r="D72" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E72" t="s">
         <v>105</v>
       </c>
       <c r="F72" t="s">
         <v>105</v>
       </c>
-      <c r="G72" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D73">
-        <v>1</v>
-      </c>
-      <c r="E73" s="2" t="s">
+      <c r="D73" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E73" t="s">
         <v>105</v>
       </c>
       <c r="F73" t="s">
         <v>105</v>
       </c>
-      <c r="G73" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D74">
-        <v>1</v>
-      </c>
-      <c r="E74" s="2" t="s">
+      <c r="D74" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E74" t="s">
         <v>105</v>
       </c>
       <c r="F74" t="s">
         <v>105</v>
       </c>
-      <c r="G74" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D75">
-        <v>1</v>
-      </c>
-      <c r="E75" s="2" t="s">
+      <c r="D75" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E75" t="s">
         <v>105</v>
       </c>
       <c r="F75" t="s">
         <v>105</v>
       </c>
-      <c r="G75" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D76">
-        <v>1</v>
-      </c>
-      <c r="E76" s="2" t="s">
+      <c r="D76" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E76" t="s">
         <v>105</v>
       </c>
       <c r="F76" t="s">
         <v>105</v>
       </c>
-      <c r="G76" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D77">
-        <v>1</v>
-      </c>
-      <c r="E77" s="2" t="s">
+      <c r="D77" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E77" t="s">
         <v>105</v>
       </c>
       <c r="F77" t="s">
         <v>105</v>
       </c>
-      <c r="G77" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D78">
-        <v>1</v>
-      </c>
-      <c r="E78" s="2" t="s">
+      <c r="D78" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E78" t="s">
         <v>105</v>
       </c>
       <c r="F78" t="s">
         <v>105</v>
       </c>
-      <c r="G78" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D79">
-        <v>1</v>
-      </c>
-      <c r="E79" s="2" t="s">
+      <c r="D79" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E79" t="s">
         <v>105</v>
       </c>
       <c r="F79" t="s">
         <v>105</v>
       </c>
-      <c r="G79" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D80">
-        <v>1</v>
-      </c>
-      <c r="E80" s="2" t="s">
+      <c r="D80" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E80" t="s">
         <v>105</v>
       </c>
       <c r="F80" t="s">
         <v>105</v>
       </c>
-      <c r="G80" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D81">
-        <v>1</v>
-      </c>
-      <c r="E81" s="2" t="s">
+      <c r="D81" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E81" t="s">
         <v>105</v>
       </c>
       <c r="F81" t="s">
         <v>105</v>
       </c>
-      <c r="G81" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D82">
-        <v>1</v>
-      </c>
-      <c r="E82" s="2" t="s">
+      <c r="D82" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E82" t="s">
         <v>105</v>
       </c>
       <c r="F82" t="s">
         <v>105</v>
       </c>
-      <c r="G82" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D83">
-        <v>1</v>
-      </c>
-      <c r="E83" s="2" t="s">
+      <c r="D83" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E83" t="s">
         <v>105</v>
       </c>
       <c r="F83" t="s">
         <v>105</v>
       </c>
-      <c r="G83" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D84">
-        <v>1</v>
-      </c>
-      <c r="E84" s="2" t="s">
+      <c r="D84" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E84" t="s">
         <v>105</v>
       </c>
       <c r="F84" t="s">
         <v>105</v>
       </c>
-      <c r="G84" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D85">
-        <v>1</v>
-      </c>
-      <c r="E85" s="2" t="s">
+      <c r="D85" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E85" t="s">
         <v>105</v>
       </c>
       <c r="F85" t="s">
         <v>105</v>
       </c>
-      <c r="G85" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D86">
-        <v>1</v>
-      </c>
-      <c r="E86" s="2" t="s">
+      <c r="D86" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E86" t="s">
         <v>105</v>
       </c>
       <c r="F86" t="s">
         <v>105</v>
       </c>
-      <c r="G86" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D87">
-        <v>1</v>
-      </c>
-      <c r="E87" s="2" t="s">
+      <c r="D87" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E87" t="s">
         <v>105</v>
       </c>
       <c r="F87" t="s">
         <v>105</v>
       </c>
-      <c r="G87" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D88">
-        <v>1</v>
-      </c>
-      <c r="E88" s="2" t="s">
+      <c r="D88" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E88" t="s">
         <v>105</v>
       </c>
       <c r="F88" t="s">
         <v>105</v>
       </c>
-      <c r="G88" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D89">
-        <v>1</v>
-      </c>
-      <c r="E89" s="2" t="s">
+      <c r="D89" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E89" t="s">
         <v>105</v>
       </c>
       <c r="F89" t="s">
         <v>105</v>
       </c>
-      <c r="G89" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D90">
-        <v>1</v>
-      </c>
-      <c r="E90" s="2" t="s">
+      <c r="D90" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E90" t="s">
         <v>105</v>
       </c>
       <c r="F90" t="s">
         <v>105</v>
       </c>
-      <c r="G90" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D91">
-        <v>1</v>
-      </c>
-      <c r="E91" s="2" t="s">
+      <c r="D91" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E91" t="s">
         <v>105</v>
       </c>
       <c r="F91" t="s">
         <v>105</v>
       </c>
-      <c r="G91" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D92">
-        <v>1</v>
-      </c>
-      <c r="E92" s="2" t="s">
+      <c r="D92" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E92" t="s">
         <v>105</v>
       </c>
       <c r="F92" t="s">
         <v>105</v>
       </c>
-      <c r="G92" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D93">
-        <v>1</v>
-      </c>
-      <c r="E93" s="2" t="s">
+      <c r="D93" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E93" t="s">
         <v>105</v>
       </c>
       <c r="F93" t="s">
         <v>105</v>
       </c>
-      <c r="G93" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D94">
-        <v>1</v>
-      </c>
-      <c r="E94" s="2" t="s">
+      <c r="D94" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E94" t="s">
         <v>105</v>
       </c>
       <c r="F94" t="s">
         <v>105</v>
       </c>
-      <c r="G94" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D95">
-        <v>1</v>
-      </c>
-      <c r="E95" s="2" t="s">
+      <c r="D95" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E95" t="s">
         <v>105</v>
       </c>
       <c r="F95" t="s">
         <v>105</v>
       </c>
-      <c r="G95" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D96">
-        <v>1</v>
-      </c>
-      <c r="E96" s="2" t="s">
+      <c r="D96" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E96" t="s">
         <v>105</v>
       </c>
       <c r="F96" t="s">
         <v>105</v>
       </c>
-      <c r="G96" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D97">
-        <v>1</v>
-      </c>
-      <c r="E97" s="2" t="s">
+      <c r="D97" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E97" t="s">
         <v>105</v>
       </c>
       <c r="F97" t="s">
         <v>105</v>
       </c>
-      <c r="G97" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D98">
-        <v>1</v>
-      </c>
-      <c r="E98" s="2" t="s">
+      <c r="D98" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E98" t="s">
         <v>105</v>
       </c>
       <c r="F98" t="s">
         <v>105</v>
       </c>
-      <c r="G98" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D99">
-        <v>1</v>
-      </c>
-      <c r="E99" s="2" t="s">
+      <c r="D99" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E99" t="s">
         <v>105</v>
       </c>
       <c r="F99" t="s">
         <v>105</v>
       </c>
-      <c r="G99" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D100">
-        <v>1</v>
-      </c>
-      <c r="E100" s="2" t="s">
+      <c r="D100" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E100" t="s">
         <v>105</v>
       </c>
       <c r="F100" t="s">
         <v>105</v>
       </c>
-      <c r="G100" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D101">
-        <v>1</v>
-      </c>
-      <c r="E101" s="2" t="s">
+      <c r="D101" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E101" t="s">
         <v>105</v>
       </c>
       <c r="F101" t="s">
         <v>105</v>
       </c>
-      <c r="G101" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>101</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D102">
-        <v>1</v>
-      </c>
-      <c r="E102" s="2" t="s">
+      <c r="D102" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E102" t="s">
         <v>105</v>
       </c>
       <c r="F102" t="s">
         <v>105</v>
       </c>
-      <c r="G102" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>102</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D103">
-        <v>1</v>
-      </c>
-      <c r="E103" s="2" t="s">
+      <c r="D103" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E103" t="s">
         <v>105</v>
       </c>
       <c r="F103" t="s">
         <v>105</v>
       </c>
-      <c r="G103" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>103</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D104">
-        <v>1</v>
-      </c>
-      <c r="E104" s="2" t="s">
+      <c r="D104" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E104" t="s">
         <v>105</v>
       </c>
       <c r="F104" t="s">
         <v>105</v>
       </c>
-      <c r="G104" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>104</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D105">
-        <v>1</v>
-      </c>
-      <c r="E105" s="2" t="s">
+      <c r="D105" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E105" t="s">
         <v>105</v>
       </c>
       <c r="F105" t="s">
         <v>105</v>
       </c>
-      <c r="G105" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D106">
-        <v>1</v>
-      </c>
-      <c r="E106" s="2" t="s">
+      <c r="D106" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E106" t="s">
         <v>105</v>
       </c>
       <c r="F106" t="s">
-        <v>105</v>
-      </c>
-      <c r="G106" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>